<commit_message>
Ready for proof stage
</commit_message>
<xml_diff>
--- a/data/gssvars.xlsx
+++ b/data/gssvars.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="codebook" sheetId="1" r:id="rId1"/>
     <sheet name="Correlation" sheetId="2" r:id="rId2"/>
     <sheet name="rq" sheetId="3" r:id="rId3"/>
     <sheet name="vars" sheetId="4" r:id="rId4"/>
+    <sheet name="results" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">codebook!$A$1:$D$118</definedName>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="161">
   <si>
     <t>Respondent Background Variables</t>
   </si>
@@ -1724,9 +1725,6 @@
     <t>Sel</t>
   </si>
   <si>
-    <t>Is there an association between opinion w.r.t. extra marital conduct and year controlling for gender?</t>
-  </si>
-  <si>
     <t>Is there an association between opinion w.r.t. extra marital conduct and region?</t>
   </si>
   <si>
@@ -1760,10 +1758,16 @@
     <t>Years</t>
   </si>
   <si>
-    <t>1972-2016</t>
-  </si>
-  <si>
     <t>2012-2016</t>
+  </si>
+  <si>
+    <t>Result</t>
+  </si>
+  <si>
+    <t>Is there a linear trend in the proportion of non-traditional opinion over time, controlling for gender?</t>
+  </si>
+  <si>
+    <t>1973-2016</t>
   </si>
 </sst>
 </file>
@@ -4150,8 +4154,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4164,10 +4168,10 @@
         <v>124</v>
       </c>
       <c r="B1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -4175,10 +4179,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>146</v>
+        <v>159</v>
       </c>
       <c r="C2" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -4186,10 +4190,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -4197,10 +4201,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C4" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -4208,10 +4212,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C5" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -4220,10 +4224,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C6" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -4232,10 +4236,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C7" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
   </sheetData>
@@ -4250,7 +4254,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
@@ -4269,7 +4273,7 @@
         <v>126</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -4280,7 +4284,7 @@
         <v>102</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -4291,7 +4295,7 @@
         <v>11</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -4302,7 +4306,7 @@
         <v>78</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -4313,7 +4317,7 @@
         <v>25</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -4324,7 +4328,7 @@
         <v>36</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -4335,7 +4339,7 @@
         <v>12</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -4346,7 +4350,7 @@
         <v>10</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -4457,4 +4461,101 @@
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="92.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B1" t="s">
+        <v>151</v>
+      </c>
+      <c r="C1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>159</v>
+      </c>
+      <c r="C2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>146</v>
+      </c>
+      <c r="C3" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>147</v>
+      </c>
+      <c r="C4" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>148</v>
+      </c>
+      <c r="C5" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <f>A5+1</f>
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>149</v>
+      </c>
+      <c r="C6" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <f t="shared" ref="A7" si="0">A6+1</f>
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>150</v>
+      </c>
+      <c r="C7" t="s">
+        <v>129</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
all but the spellcheck
</commit_message>
<xml_diff>
--- a/data/gssvars.xlsx
+++ b/data/gssvars.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="codebook" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="results" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">codebook!$A$1:$D$118</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">codebook!$B$1:$E$118</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="676" uniqueCount="174">
   <si>
     <t>Respondent Background Variables</t>
   </si>
@@ -1677,9 +1677,6 @@
     <t>Yes</t>
   </si>
   <si>
-    <t>Downloaded</t>
-  </si>
-  <si>
     <t>tvhours</t>
   </si>
   <si>
@@ -1768,6 +1765,48 @@
   </si>
   <si>
     <t>1973-2016</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>Coursera</t>
+  </si>
+  <si>
+    <t>GSS</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Cases</t>
+  </si>
+  <si>
+    <t>Number of brothers and sisters</t>
+  </si>
+  <si>
+    <t>SIBS</t>
+  </si>
+  <si>
+    <t>rincome</t>
+  </si>
+  <si>
+    <t>Respondents Income</t>
+  </si>
+  <si>
+    <t>About how often did you have sex during the last 12 months?</t>
+  </si>
+  <si>
+    <t>sexfreq</t>
+  </si>
+  <si>
+    <t>evstray</t>
+  </si>
+  <si>
+    <t>Have sex other than spouse while married</t>
+  </si>
+  <si>
+    <t>sibs</t>
   </si>
 </sst>
 </file>
@@ -2128,1813 +2167,2484 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E171"/>
+  <dimension ref="A1:F157"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="D123" sqref="D123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="9.140625" style="2"/>
-    <col min="4" max="4" width="49.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="4" width="9.140625" style="2"/>
+    <col min="5" max="5" width="49.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" s="2" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B2" s="2">
+        <v>161</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C2" s="2">
         <v>1</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="E2" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="B3" s="2">
+        <v>161</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C3" s="2">
         <v>2</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="E3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="7">
-        <v>43036</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="B4" s="2">
+        <v>161</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C4" s="2">
         <v>3</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="E4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="7">
-        <v>43036</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="B5" s="2">
+        <v>161</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C5" s="2">
         <v>4</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="D5" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="E5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="7">
-        <v>43036</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B6" s="2">
+        <v>161</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C6" s="2">
         <v>5</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="D6" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="E6" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B7" s="2">
+        <v>161</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C7" s="2">
         <v>6</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="D7" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="E7" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B8" s="2">
+        <v>161</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C8" s="2">
         <v>7</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="D8" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="E8" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="B9" s="2">
+        <v>161</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C9" s="2">
         <v>8</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="D9" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="E9" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E9" s="7">
-        <v>43036</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B10" s="2">
+        <v>161</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C10" s="2">
         <v>9</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="D10" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="E10" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B11" s="2">
+        <v>161</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C11" s="2">
         <v>10</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="D11" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="E11" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B12" s="2">
+        <v>161</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C12" s="2">
         <v>11</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="D12" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="E12" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B13" s="2">
+        <v>161</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C13" s="2">
         <v>12</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="D13" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="E13" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B14" s="2">
+        <v>161</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C14" s="2">
         <v>13</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="D14" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="E14" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B15" s="2">
+        <v>161</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C15" s="2">
         <v>14</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="D15" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="E15" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B16" s="2">
+        <v>161</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C16" s="2">
         <v>15</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="D16" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="E16" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B17" s="2">
+        <v>161</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C17" s="2">
         <v>16</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="D17" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="E17" s="2" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="B18" s="2">
+        <v>161</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C18" s="2">
         <v>17</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="D18" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="E18" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="E18" s="7">
-        <v>43036</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B19" s="2">
+        <v>161</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C19" s="2">
         <v>18</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="D19" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="E19" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B20" s="2">
+        <v>161</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C20" s="2">
         <v>19</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="D20" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D20" s="5" t="s">
+      <c r="E20" s="2" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B21" s="2">
+        <v>161</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C21" s="2">
         <v>20</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="D21" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D21" s="5" t="s">
+      <c r="E21" s="2" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B22" s="2">
+        <v>161</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C22" s="2">
         <v>21</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="D22" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D22" s="5" t="s">
+      <c r="E22" s="2" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B23" s="2">
+        <v>161</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C23" s="2">
         <v>22</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="D23" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D23" s="5" t="s">
+      <c r="E23" s="2" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B24" s="2">
+        <v>161</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C24" s="2">
         <v>23</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="D24" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D24" s="5" t="s">
+      <c r="E24" s="2" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B25" s="2">
+        <v>161</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C25" s="2">
         <v>24</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="D25" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D25" s="5" t="s">
+      <c r="E25" s="2" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B26" s="2">
+        <v>161</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C26" s="2">
         <v>25</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="D26" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D26" s="5" t="s">
+      <c r="E26" s="2" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B27" s="2">
+        <v>161</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C27" s="2">
         <v>26</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="D27" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D27" s="5" t="s">
+      <c r="E27" s="2" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B28" s="2">
+        <v>161</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C28" s="2">
         <v>27</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="D28" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D28" s="5" t="s">
+      <c r="E28" s="2" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="B29" s="2">
+        <v>161</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C29" s="2">
         <v>28</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="D29" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D29" s="5" t="s">
+      <c r="E29" s="2" t="s">
         <v>36</v>
-      </c>
-      <c r="E29" s="7">
-        <v>43036</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="B30" s="2">
+        <v>161</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C30" s="2">
         <v>29</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="D30" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D30" s="5" t="s">
+      <c r="E30" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="E30" s="7">
-        <v>43036</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B31" s="2">
+        <v>161</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C31" s="2">
         <v>30</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="D31" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D31" s="5" t="s">
+      <c r="E31" s="2" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B32" s="2">
+        <v>161</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C32" s="2">
         <v>31</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="D32" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D32" s="5" t="s">
+      <c r="E32" s="2" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B33" s="2">
+        <v>161</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C33" s="2">
         <v>32</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="D33" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D33" s="5" t="s">
+      <c r="E33" s="2" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B34" s="2">
+        <v>161</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C34" s="2">
         <v>33</v>
       </c>
-      <c r="C34" s="2" t="s">
+      <c r="D34" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D34" s="5" t="s">
+      <c r="E34" s="2" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B35" s="2">
+        <v>161</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C35" s="2">
         <v>34</v>
       </c>
-      <c r="C35" s="2" t="s">
+      <c r="D35" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D35" s="5" t="s">
+      <c r="E35" s="2" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B36" s="2">
+        <v>161</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C36" s="2">
         <v>35</v>
       </c>
-      <c r="C36" s="2" t="s">
+      <c r="D36" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D36" s="5" t="s">
+      <c r="E36" s="2" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B37" s="2">
+        <v>161</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C37" s="2">
         <v>36</v>
       </c>
-      <c r="C37" s="2" t="s">
+      <c r="D37" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D37" s="5" t="s">
+      <c r="E37" s="2" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B38" s="2">
+        <v>161</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C38" s="2">
         <v>37</v>
       </c>
-      <c r="C38" s="2" t="s">
+      <c r="D38" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D38" s="5" t="s">
+      <c r="E38" s="2" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B39" s="2">
+        <v>161</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C39" s="2">
         <v>38</v>
       </c>
-      <c r="C39" s="2" t="s">
+      <c r="D39" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D39" s="5" t="s">
+      <c r="E39" s="2" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B40" s="2">
+        <v>161</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C40" s="2">
         <v>39</v>
       </c>
-      <c r="C40" s="2" t="s">
+      <c r="D40" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D40" s="5" t="s">
+      <c r="E40" s="2" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B41" s="2">
+        <v>161</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C41" s="2">
         <v>40</v>
       </c>
-      <c r="C41" s="2" t="s">
+      <c r="D41" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D41" s="5" t="s">
+      <c r="E41" s="2" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B42" s="2">
+        <v>161</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C42" s="2">
         <v>41</v>
       </c>
-      <c r="C42" s="2" t="s">
+      <c r="D42" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D42" s="5" t="s">
+      <c r="E42" s="2" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B43" s="2">
+        <v>161</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C43" s="2">
         <v>42</v>
       </c>
-      <c r="C43" s="2" t="s">
+      <c r="D43" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D43" s="5" t="s">
+      <c r="E43" s="2" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B44" s="2">
+        <v>161</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C44" s="2">
         <v>43</v>
       </c>
-      <c r="C44" s="2" t="s">
+      <c r="D44" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D44" s="5" t="s">
+      <c r="E44" s="2" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B45" s="2">
+        <v>161</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C45" s="2">
         <v>44</v>
       </c>
-      <c r="C45" s="2" t="s">
+      <c r="D45" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D45" s="5" t="s">
+      <c r="E45" s="2" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B46" s="2">
+        <v>161</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C46" s="2">
         <v>45</v>
       </c>
-      <c r="C46" s="2" t="s">
+      <c r="D46" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D46" s="5" t="s">
+      <c r="E46" s="2" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="B47" s="2">
+        <v>161</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C47" s="2">
         <v>46</v>
       </c>
-      <c r="C47" s="2" t="s">
+      <c r="D47" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D47" s="5" t="s">
+      <c r="E47" s="2" t="s">
         <v>54</v>
-      </c>
-      <c r="E47" s="7">
-        <v>43036</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="B48" s="2">
+        <v>161</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C48" s="2">
         <v>47</v>
       </c>
-      <c r="C48" s="2" t="s">
+      <c r="D48" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D48" s="5" t="s">
+      <c r="E48" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="E48" s="7">
-        <v>43036</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B49" s="2">
+        <v>161</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C49" s="2">
         <v>48</v>
       </c>
-      <c r="C49" s="2" t="s">
+      <c r="D49" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D49" s="5" t="s">
+      <c r="E49" s="2" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B50" s="2">
+        <v>161</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C50" s="2">
         <v>49</v>
       </c>
-      <c r="C50" s="2" t="s">
+      <c r="D50" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D50" s="5" t="s">
+      <c r="E50" s="2" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B51" s="2">
+        <v>161</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C51" s="2">
         <v>50</v>
       </c>
-      <c r="C51" s="2" t="s">
+      <c r="D51" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D51" s="5" t="s">
+      <c r="E51" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B52" s="2">
+        <v>161</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C52" s="2">
         <v>51</v>
       </c>
-      <c r="C52" s="2" t="s">
+      <c r="D52" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D52" s="5" t="s">
+      <c r="E52" s="2" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B53" s="2">
+        <v>161</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C53" s="2">
         <v>52</v>
       </c>
-      <c r="C53" s="2" t="s">
+      <c r="D53" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D53" s="5" t="s">
+      <c r="E53" s="2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B54" s="2">
+        <v>161</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C54" s="2">
         <v>53</v>
       </c>
-      <c r="C54" s="2" t="s">
+      <c r="D54" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D54" s="5" t="s">
+      <c r="E54" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B55" s="2">
+        <v>161</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C55" s="2">
         <v>54</v>
       </c>
-      <c r="C55" s="2" t="s">
+      <c r="D55" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D55" s="5" t="s">
+      <c r="E55" s="2" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B56" s="2">
+        <v>161</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C56" s="2">
         <v>55</v>
       </c>
-      <c r="C56" s="2" t="s">
+      <c r="D56" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D56" s="5" t="s">
+      <c r="E56" s="2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B57" s="2">
+        <v>161</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C57" s="2">
         <v>56</v>
       </c>
-      <c r="C57" s="2" t="s">
+      <c r="D57" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D57" s="5" t="s">
+      <c r="E57" s="2" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B58" s="2">
+        <v>161</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C58" s="2">
         <v>57</v>
       </c>
-      <c r="C58" s="2" t="s">
+      <c r="D58" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D58" s="5" t="s">
+      <c r="E58" s="2" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B59" s="2">
+        <v>161</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C59" s="2">
         <v>58</v>
       </c>
-      <c r="C59" s="2" t="s">
+      <c r="D59" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D59" s="5" t="s">
+      <c r="E59" s="2" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B60" s="2">
+        <v>161</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C60" s="2">
         <v>59</v>
       </c>
-      <c r="C60" s="2" t="s">
+      <c r="D60" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D60" s="5" t="s">
+      <c r="E60" s="2" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B61" s="2">
+        <v>161</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C61" s="2">
         <v>60</v>
       </c>
-      <c r="C61" s="2" t="s">
+      <c r="D61" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D61" s="5" t="s">
+      <c r="E61" s="2" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B62" s="2">
+        <v>161</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C62" s="2">
         <v>61</v>
       </c>
-      <c r="C62" s="2" t="s">
+      <c r="D62" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D62" s="5" t="s">
+      <c r="E62" s="2" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B63" s="2">
+        <v>161</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C63" s="2">
         <v>62</v>
       </c>
-      <c r="C63" s="2" t="s">
+      <c r="D63" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D63" s="5" t="s">
+      <c r="E63" s="2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B64" s="2">
+        <v>161</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C64" s="2">
         <v>63</v>
       </c>
-      <c r="C64" s="2" t="s">
+      <c r="D64" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D64" s="5" t="s">
+      <c r="E64" s="2" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B65" s="2">
+        <v>161</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C65" s="2">
         <v>64</v>
       </c>
-      <c r="C65" s="2" t="s">
+      <c r="D65" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D65" s="5" t="s">
+      <c r="E65" s="2" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B66" s="2">
+        <v>161</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C66" s="2">
         <v>65</v>
       </c>
-      <c r="C66" s="2" t="s">
+      <c r="D66" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D66" s="5" t="s">
+      <c r="E66" s="2" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B67" s="2">
+        <v>161</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C67" s="2">
         <v>66</v>
       </c>
-      <c r="C67" s="2" t="s">
+      <c r="D67" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D67" s="5" t="s">
+      <c r="E67" s="2" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B68" s="2">
+        <v>161</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C68" s="2">
         <v>67</v>
       </c>
-      <c r="C68" s="2" t="s">
+      <c r="D68" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D68" s="5" t="s">
+      <c r="E68" s="2" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B69" s="2">
+        <v>161</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C69" s="2">
         <v>68</v>
       </c>
-      <c r="C69" s="2" t="s">
+      <c r="D69" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D69" s="5" t="s">
+      <c r="E69" s="2" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B70" s="2">
+        <v>161</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C70" s="2">
         <v>69</v>
       </c>
-      <c r="C70" s="2" t="s">
+      <c r="D70" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D70" s="5" t="s">
+      <c r="E70" s="2" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="B71" s="2">
+        <v>161</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C71" s="2">
         <v>70</v>
       </c>
-      <c r="C71" s="2" t="s">
+      <c r="D71" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D71" s="5" t="s">
+      <c r="E71" s="2" t="s">
         <v>78</v>
-      </c>
-      <c r="E71" s="7">
-        <v>43036</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B72" s="2">
+        <v>161</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C72" s="2">
         <v>71</v>
       </c>
-      <c r="C72" s="2" t="s">
+      <c r="D72" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D72" s="5" t="s">
+      <c r="E72" s="2" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="B73" s="2">
+        <v>161</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C73" s="2">
         <v>72</v>
       </c>
-      <c r="C73" s="2" t="s">
+      <c r="D73" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D73" s="5" t="s">
+      <c r="E73" s="2" t="s">
         <v>80</v>
-      </c>
-      <c r="E73" s="7">
-        <v>43036</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B74" s="2">
+        <v>161</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C74" s="2">
         <v>73</v>
       </c>
-      <c r="C74" s="2" t="s">
+      <c r="D74" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D74" s="5" t="s">
+      <c r="E74" s="2" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B75" s="2">
+        <v>161</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C75" s="2">
         <v>74</v>
       </c>
-      <c r="C75" s="2" t="s">
+      <c r="D75" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D75" s="5" t="s">
+      <c r="E75" s="2" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B76" s="2">
+        <v>161</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C76" s="2">
         <v>75</v>
       </c>
-      <c r="C76" s="2" t="s">
+      <c r="D76" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D76" s="5" t="s">
+      <c r="E76" s="2" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B77" s="2">
+        <v>161</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C77" s="2">
         <v>76</v>
       </c>
-      <c r="C77" s="2" t="s">
+      <c r="D77" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D77" s="5" t="s">
+      <c r="E77" s="2" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B78" s="2">
+        <v>161</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C78" s="2">
         <v>77</v>
       </c>
-      <c r="C78" s="2" t="s">
+      <c r="D78" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D78" s="5" t="s">
+      <c r="E78" s="2" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B79" s="2">
+        <v>161</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C79" s="2">
         <v>78</v>
       </c>
-      <c r="C79" s="2" t="s">
+      <c r="D79" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D79" s="5" t="s">
+      <c r="E79" s="2" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B80" s="2">
+        <v>161</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C80" s="2">
         <v>79</v>
       </c>
-      <c r="C80" s="2" t="s">
+      <c r="D80" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D80" s="5" t="s">
+      <c r="E80" s="2" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B81" s="2">
+        <v>161</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C81" s="2">
         <v>80</v>
       </c>
-      <c r="C81" s="2" t="s">
+      <c r="D81" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D81" s="5" t="s">
+      <c r="E81" s="2" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B82" s="2">
+        <v>161</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C82" s="2">
         <v>81</v>
       </c>
-      <c r="C82" s="2" t="s">
+      <c r="D82" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D82" s="5" t="s">
+      <c r="E82" s="2" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B83" s="2">
+        <v>161</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C83" s="2">
         <v>82</v>
       </c>
-      <c r="C83" s="2" t="s">
+      <c r="D83" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D83" s="5" t="s">
+      <c r="E83" s="2" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B84" s="2">
+        <v>161</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C84" s="2">
         <v>83</v>
       </c>
-      <c r="C84" s="2" t="s">
+      <c r="D84" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D84" s="5" t="s">
+      <c r="E84" s="2" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B85" s="2">
+        <v>161</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C85" s="2">
         <v>84</v>
       </c>
-      <c r="C85" s="2" t="s">
+      <c r="D85" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D85" s="5" t="s">
+      <c r="E85" s="2" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B86" s="2">
+        <v>161</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C86" s="2">
         <v>85</v>
       </c>
-      <c r="C86" s="2" t="s">
+      <c r="D86" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D86" s="5" t="s">
+      <c r="E86" s="2" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B87" s="2">
+        <v>161</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C87" s="2">
         <v>86</v>
       </c>
-      <c r="C87" s="2" t="s">
+      <c r="D87" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D87" s="5" t="s">
+      <c r="E87" s="2" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B88" s="2">
+        <v>161</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C88" s="2">
         <v>87</v>
       </c>
-      <c r="C88" s="2" t="s">
+      <c r="D88" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D88" s="5" t="s">
+      <c r="E88" s="2" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B89" s="2">
+        <v>161</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C89" s="2">
         <v>88</v>
       </c>
-      <c r="C89" s="2" t="s">
+      <c r="D89" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D89" s="5" t="s">
+      <c r="E89" s="2" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B90" s="2">
+        <v>161</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C90" s="2">
         <v>89</v>
       </c>
-      <c r="C90" s="2" t="s">
+      <c r="D90" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D90" s="5" t="s">
+      <c r="E90" s="2" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B91" s="2">
+        <v>161</v>
+      </c>
+      <c r="B91" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C91" s="2">
         <v>90</v>
       </c>
-      <c r="C91" s="2" t="s">
+      <c r="D91" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D91" s="5" t="s">
+      <c r="E91" s="2" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B92" s="2">
+        <v>161</v>
+      </c>
+      <c r="B92" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C92" s="2">
         <v>91</v>
       </c>
-      <c r="C92" s="2" t="s">
+      <c r="D92" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D92" s="5" t="s">
+      <c r="E92" s="2" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B93" s="2">
+        <v>161</v>
+      </c>
+      <c r="B93" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C93" s="2">
         <v>92</v>
       </c>
-      <c r="C93" s="2" t="s">
+      <c r="D93" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D93" s="5" t="s">
+      <c r="E93" s="2" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B94" s="2">
+        <v>161</v>
+      </c>
+      <c r="B94" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C94" s="2">
         <v>93</v>
       </c>
-      <c r="C94" s="2" t="s">
+      <c r="D94" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D94" s="5" t="s">
+      <c r="E94" s="2" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="B95" s="2">
+        <v>161</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C95" s="2">
         <v>94</v>
       </c>
-      <c r="C95" s="2" t="s">
+      <c r="D95" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D95" s="5" t="s">
+      <c r="E95" s="2" t="s">
         <v>102</v>
-      </c>
-      <c r="E95" s="7">
-        <v>43036</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B96" s="2">
+        <v>161</v>
+      </c>
+      <c r="B96" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C96" s="2">
         <v>95</v>
       </c>
-      <c r="C96" s="2" t="s">
+      <c r="D96" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D96" s="5" t="s">
+      <c r="E96" s="2" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B97" s="2">
+        <v>161</v>
+      </c>
+      <c r="B97" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C97" s="2">
         <v>96</v>
       </c>
-      <c r="C97" s="2" t="s">
+      <c r="D97" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D97" s="5" t="s">
+      <c r="E97" s="2" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B98" s="2">
+        <v>161</v>
+      </c>
+      <c r="B98" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C98" s="2">
         <v>97</v>
       </c>
-      <c r="C98" s="2" t="s">
+      <c r="D98" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D98" s="5" t="s">
+      <c r="E98" s="2" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B99" s="2">
+        <v>161</v>
+      </c>
+      <c r="B99" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C99" s="2">
         <v>98</v>
       </c>
-      <c r="C99" s="2" t="s">
+      <c r="D99" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D99" s="5" t="s">
+      <c r="E99" s="2" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B100" s="2">
+        <v>161</v>
+      </c>
+      <c r="B100" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C100" s="2">
         <v>99</v>
       </c>
-      <c r="C100" s="2" t="s">
+      <c r="D100" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D100" s="5" t="s">
+      <c r="E100" s="2" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B101" s="2">
+        <v>161</v>
+      </c>
+      <c r="B101" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C101" s="2">
         <v>100</v>
       </c>
-      <c r="C101" s="2" t="s">
+      <c r="D101" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D101" s="5" t="s">
+      <c r="E101" s="2" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B102" s="2">
+        <v>161</v>
+      </c>
+      <c r="B102" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C102" s="2">
         <v>101</v>
       </c>
-      <c r="C102" s="2" t="s">
+      <c r="D102" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D102" s="5" t="s">
+      <c r="E102" s="2" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B103" s="2">
+        <v>161</v>
+      </c>
+      <c r="B103" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C103" s="2">
         <v>102</v>
       </c>
-      <c r="C103" s="2" t="s">
+      <c r="D103" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D103" s="5" t="s">
+      <c r="E103" s="2" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B104" s="2">
+        <v>161</v>
+      </c>
+      <c r="B104" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C104" s="2">
         <v>103</v>
       </c>
-      <c r="C104" s="2" t="s">
+      <c r="D104" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D104" s="5" t="s">
+      <c r="E104" s="2" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B105" s="2">
+        <v>161</v>
+      </c>
+      <c r="B105" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C105" s="2">
         <v>104</v>
       </c>
-      <c r="C105" s="2" t="s">
+      <c r="D105" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D105" s="5" t="s">
+      <c r="E105" s="2" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B106" s="2">
+        <v>161</v>
+      </c>
+      <c r="B106" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C106" s="2">
         <v>105</v>
       </c>
-      <c r="C106" s="2" t="s">
+      <c r="D106" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B107" s="2">
+        <v>161</v>
+      </c>
+      <c r="B107" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C107" s="2">
         <v>106</v>
       </c>
-      <c r="C107" s="2" t="s">
+      <c r="D107" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D107" s="6" t="s">
+      <c r="E107" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B108" s="2">
+        <v>161</v>
+      </c>
+      <c r="B108" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C108" s="2">
         <v>107</v>
       </c>
-      <c r="C108" s="2" t="s">
+      <c r="D108" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D108" s="4"/>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B109" s="2">
+        <v>161</v>
+      </c>
+      <c r="B109" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C109" s="2">
         <v>108</v>
       </c>
-      <c r="C109" s="2" t="s">
+      <c r="D109" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D109" s="5" t="s">
+      <c r="E109" s="2" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="B110" s="2">
+        <v>161</v>
+      </c>
+      <c r="B110" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C110" s="2">
         <v>109</v>
       </c>
-      <c r="C110" s="2" t="s">
+      <c r="D110" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D110" s="5" t="s">
+      <c r="E110" s="2" t="s">
         <v>114</v>
-      </c>
-      <c r="E110" s="7">
-        <v>43036</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B111" s="2">
+        <v>161</v>
+      </c>
+      <c r="B111" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C111" s="2">
         <v>110</v>
       </c>
-      <c r="C111" s="2" t="s">
+      <c r="D111" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D111" s="5" t="s">
+      <c r="E111" s="2" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B112" s="2">
+        <v>161</v>
+      </c>
+      <c r="B112" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C112" s="2">
         <v>111</v>
       </c>
-      <c r="C112" s="2" t="s">
+      <c r="D112" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D112" s="5" t="s">
+      <c r="E112" s="2" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B113" s="2">
+        <v>161</v>
+      </c>
+      <c r="B113" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C113" s="2">
         <v>112</v>
       </c>
-      <c r="C113" s="2" t="s">
+      <c r="D113" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D113" s="5" t="s">
+      <c r="E113" s="2" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B114" s="2">
+        <v>161</v>
+      </c>
+      <c r="B114" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C114" s="2">
         <v>113</v>
       </c>
-      <c r="C114" s="2" t="s">
+      <c r="D114" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D114" s="5" t="s">
+      <c r="E114" s="2" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B115" s="2">
+        <v>161</v>
+      </c>
+      <c r="B115" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C115" s="2">
         <v>114</v>
       </c>
-      <c r="C115" s="2" t="s">
+      <c r="D115" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D115" s="5" t="s">
+      <c r="E115" s="2" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B116" s="2">
+        <v>161</v>
+      </c>
+      <c r="B116" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C116" s="2">
         <v>115</v>
       </c>
-      <c r="C116" s="2" t="s">
+      <c r="D116" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D116" s="5" t="s">
+      <c r="E116" s="2" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B117" s="2">
+        <v>161</v>
+      </c>
+      <c r="B117" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C117" s="2">
         <v>116</v>
       </c>
-      <c r="C117" s="2" t="s">
+      <c r="D117" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D117" s="5" t="s">
+      <c r="E117" s="2" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B118" s="2">
+        <v>161</v>
+      </c>
+      <c r="B118" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C118" s="2">
         <v>117</v>
       </c>
-      <c r="C118" s="2" t="s">
+      <c r="D118" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D118" s="5" t="s">
+      <c r="E118" s="2" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D119" s="1"/>
-    </row>
-    <row r="121" spans="1:4" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="D121" s="3"/>
-    </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D122" s="4"/>
-    </row>
-    <row r="124" spans="1:4" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="D124" s="3"/>
-    </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D125" s="4"/>
-    </row>
-    <row r="127" spans="1:4" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="D127" s="3"/>
-    </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D128" s="4"/>
-    </row>
-    <row r="130" spans="4:4" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="D130" s="3"/>
-    </row>
-    <row r="132" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D132" s="6"/>
-    </row>
-    <row r="133" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D133" s="4"/>
-    </row>
-    <row r="135" spans="4:4" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="D135" s="3"/>
-    </row>
-    <row r="136" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D136" s="4"/>
-    </row>
-    <row r="138" spans="4:4" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="D138" s="3"/>
-    </row>
-    <row r="140" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D140" s="6"/>
-    </row>
-    <row r="141" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D141" s="4"/>
-    </row>
-    <row r="143" spans="4:4" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="D143" s="3"/>
-    </row>
-    <row r="145" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D145" s="6"/>
-    </row>
-    <row r="146" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D146" s="4"/>
-    </row>
-    <row r="148" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D148" s="6"/>
-    </row>
-    <row r="149" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D149" s="4"/>
-    </row>
-    <row r="151" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D151" s="6"/>
-    </row>
-    <row r="152" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D152" s="4"/>
-    </row>
-    <row r="154" spans="4:4" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="D154" s="3"/>
-    </row>
-    <row r="156" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D156" s="6"/>
-    </row>
-    <row r="157" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D157" s="4"/>
-    </row>
-    <row r="159" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D159" s="6"/>
-    </row>
-    <row r="160" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D160" s="4"/>
-    </row>
-    <row r="162" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D162" s="6"/>
-    </row>
-    <row r="163" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D163" s="4"/>
-    </row>
-    <row r="165" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D165" s="6"/>
-    </row>
-    <row r="166" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D166" s="4"/>
-    </row>
-    <row r="168" spans="4:4" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="D168" s="3"/>
-    </row>
-    <row r="170" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D170" s="6"/>
-    </row>
-    <row r="171" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D171" s="4"/>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A119" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B119" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C119" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="D119" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="E119" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="F119" s="2">
+        <v>60775</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A120" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B120" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C120" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="D120" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="E120" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="F120" s="2">
+        <v>36473</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A121" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B121" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C121" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="D121" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="E121" s="2" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A122" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B122" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C122" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="D122" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="E122" s="2" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A123" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B123" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C123" s="2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A124" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B124" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C124" s="2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A125" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B125" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C125" s="2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A126" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B126" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C126" s="2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A127" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B127" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C127" s="2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A128" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B128" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C128" s="2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A129" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B129" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C129" s="2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A130" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B130" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C130" s="2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A131" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B131" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C131" s="2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A132" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B132" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C132" s="2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A133" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B133" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C133" s="2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A134" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B134" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C134" s="2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A135" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B135" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C135" s="2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A136" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B136" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C136" s="2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A137" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B137" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C137" s="2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A138" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B138" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C138" s="2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A139" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B139" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C139" s="2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A140" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B140" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C140" s="2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A141" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B141" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C141" s="2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A142" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B142" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C142" s="2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A143" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B143" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C143" s="2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A144" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B144" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C144" s="2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A145" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B145" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C145" s="2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A146" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B146" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C146" s="2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A147" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B147" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C147" s="2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A148" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B148" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C148" s="2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A149" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B149" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C149" s="2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A150" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B150" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C150" s="2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A151" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B151" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C151" s="2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A152" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B152" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C152" s="2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A153" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B153" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C153" s="2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A154" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B154" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C154" s="2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A155" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B155" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C155" s="2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A156" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B156" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C156" s="2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A157" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B157" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C157" s="2" t="s">
+        <v>163</v>
+      </c>
     </row>
   </sheetData>
-  <sortState ref="B1:E173">
-    <sortCondition ref="B1:B173"/>
+  <sortState ref="C1:F173">
+    <sortCondition ref="C1:C173"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3943,34 +4653,34 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D1" t="s">
         <v>144</v>
-      </c>
-      <c r="D1" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B2">
         <v>8.4343190999999998E-2</v>
       </c>
       <c r="C2">
-        <f t="shared" ref="C2:C13" si="0">ABS(B2)</f>
+        <f>ABS(B2)</f>
         <v>8.4343190999999998E-2</v>
       </c>
       <c r="D2" t="s">
@@ -3979,13 +4689,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B3">
         <v>-3.6141662099999999E-2</v>
       </c>
       <c r="C3">
-        <f t="shared" si="0"/>
+        <f>ABS(B3)</f>
         <v>3.6141662099999999E-2</v>
       </c>
       <c r="D3" t="s">
@@ -3994,13 +4704,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B4">
         <v>-3.2213529999999997E-2</v>
       </c>
       <c r="C4">
-        <f t="shared" si="0"/>
+        <f>ABS(B4)</f>
         <v>3.2213529999999997E-2</v>
       </c>
       <c r="D4" t="s">
@@ -4009,13 +4719,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B5">
         <v>-3.163966E-2</v>
       </c>
       <c r="C5">
-        <f t="shared" si="0"/>
+        <f>ABS(B5)</f>
         <v>3.163966E-2</v>
       </c>
       <c r="D5" t="s">
@@ -4024,17 +4734,14 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>141</v>
+        <v>171</v>
       </c>
       <c r="B6">
-        <v>3.0346855999999998E-2</v>
+        <v>-3.0391999999999999E-2</v>
       </c>
       <c r="C6">
-        <f t="shared" si="0"/>
-        <v>3.0346855999999998E-2</v>
-      </c>
-      <c r="D6" t="s">
-        <v>129</v>
+        <f>ABS(B6)</f>
+        <v>3.0391999999999999E-2</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -4042,11 +4749,11 @@
         <v>140</v>
       </c>
       <c r="B7">
-        <v>2.6649749E-2</v>
+        <v>3.0346855999999998E-2</v>
       </c>
       <c r="C7">
-        <f t="shared" si="0"/>
-        <v>2.6649749E-2</v>
+        <f>ABS(B7)</f>
+        <v>3.0346855999999998E-2</v>
       </c>
       <c r="D7" t="s">
         <v>129</v>
@@ -4054,44 +4761,38 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>137</v>
+        <v>173</v>
       </c>
       <c r="B8">
-        <v>2.4819702999999999E-2</v>
+        <v>2.9398980000000002E-2</v>
       </c>
       <c r="C8">
-        <f t="shared" si="0"/>
-        <v>2.4819702999999999E-2</v>
-      </c>
-      <c r="D8" t="s">
-        <v>129</v>
+        <f>ABS(B8)</f>
+        <v>2.9398980000000002E-2</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>138</v>
+        <v>170</v>
       </c>
       <c r="B9">
-        <v>-1.9202296000000001E-2</v>
+        <v>-2.7596119999999998E-2</v>
       </c>
       <c r="C9">
-        <f t="shared" si="0"/>
-        <v>1.9202296000000001E-2</v>
-      </c>
-      <c r="D9" t="s">
-        <v>129</v>
+        <f>ABS(B9)</f>
+        <v>2.7596119999999998E-2</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="B10">
-        <v>-1.1525909799999999E-2</v>
+        <v>2.6649749E-2</v>
       </c>
       <c r="C10">
-        <f t="shared" si="0"/>
-        <v>1.1525909799999999E-2</v>
+        <f>ABS(B10)</f>
+        <v>2.6649749E-2</v>
       </c>
       <c r="D10" t="s">
         <v>129</v>
@@ -4102,11 +4803,11 @@
         <v>136</v>
       </c>
       <c r="B11">
-        <v>-5.7468650000000003E-3</v>
+        <v>2.4819702999999999E-2</v>
       </c>
       <c r="C11">
-        <f t="shared" si="0"/>
-        <v>5.7468650000000003E-3</v>
+        <f>ABS(B11)</f>
+        <v>2.4819702999999999E-2</v>
       </c>
       <c r="D11" t="s">
         <v>129</v>
@@ -4114,37 +4815,106 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="B12">
-        <v>-1.9329950000000001E-3</v>
+        <v>-1.985862E-2</v>
       </c>
       <c r="C12">
-        <f t="shared" si="0"/>
-        <v>1.9329950000000001E-3</v>
-      </c>
-      <c r="D12" t="s">
-        <v>129</v>
+        <f>ABS(B12)</f>
+        <v>1.985862E-2</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="B13">
+        <v>-1.9202296000000001E-2</v>
+      </c>
+      <c r="C13">
+        <f>ABS(B13)</f>
+        <v>1.9202296000000001E-2</v>
+      </c>
+      <c r="D13" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>167</v>
+      </c>
+      <c r="B14">
+        <v>1.43818E-2</v>
+      </c>
+      <c r="C14">
+        <f>ABS(B14)</f>
+        <v>1.43818E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>130</v>
+      </c>
+      <c r="B15">
+        <v>-1.1525909799999999E-2</v>
+      </c>
+      <c r="C15">
+        <f>ABS(B15)</f>
+        <v>1.1525909799999999E-2</v>
+      </c>
+      <c r="D15" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>135</v>
+      </c>
+      <c r="B16">
+        <v>-5.7468650000000003E-3</v>
+      </c>
+      <c r="C16">
+        <f>ABS(B16)</f>
+        <v>5.7468650000000003E-3</v>
+      </c>
+      <c r="D16" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>138</v>
+      </c>
+      <c r="B17">
+        <v>-1.9329950000000001E-3</v>
+      </c>
+      <c r="C17">
+        <f>ABS(B17)</f>
+        <v>1.9329950000000001E-3</v>
+      </c>
+      <c r="D17" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>132</v>
+      </c>
+      <c r="B18">
         <v>-5.0629530000000002E-4</v>
       </c>
-      <c r="C13">
-        <f t="shared" si="0"/>
+      <c r="C18">
+        <f>ABS(B18)</f>
         <v>5.0629530000000002E-4</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D18" t="s">
         <v>128</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:C15">
-    <sortCondition descending="1" ref="C2:C15"/>
+  <sortState ref="A2:D18">
+    <sortCondition descending="1" ref="C2:C18"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4154,7 +4924,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -4168,10 +4938,10 @@
         <v>124</v>
       </c>
       <c r="B1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -4179,10 +4949,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>158</v>
+      </c>
+      <c r="C2" t="s">
         <v>159</v>
-      </c>
-      <c r="C2" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -4190,10 +4960,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -4201,10 +4971,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -4212,10 +4982,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -4224,10 +4994,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C6" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -4236,10 +5006,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
   </sheetData>
@@ -4273,7 +5043,7 @@
         <v>126</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -4284,7 +5054,7 @@
         <v>102</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -4295,7 +5065,7 @@
         <v>11</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -4306,7 +5076,7 @@
         <v>78</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -4317,7 +5087,7 @@
         <v>25</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -4328,7 +5098,7 @@
         <v>36</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -4339,7 +5109,7 @@
         <v>12</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -4350,7 +5120,7 @@
         <v>10</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -4481,10 +5251,10 @@
         <v>124</v>
       </c>
       <c r="B1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -4492,7 +5262,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C2" t="s">
         <v>129</v>
@@ -4503,7 +5273,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C3" t="s">
         <v>129</v>
@@ -4514,7 +5284,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C4" t="s">
         <v>128</v>
@@ -4525,7 +5295,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C5" t="s">
         <v>129</v>
@@ -4537,7 +5307,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C6" t="s">
         <v>129</v>
@@ -4549,7 +5319,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C7" t="s">
         <v>129</v>

</xml_diff>